<commit_message>
change master -> hsy0414
</commit_message>
<xml_diff>
--- a/The Eternals/FrameDirectX12/Bin/Resource/ResourceStage/DynamicMesh/NPC/Aman_boy/AnimationInfo.xlsx
+++ b/The Eternals/FrameDirectX12/Bin/Resource/ResourceStage/DynamicMesh/NPC/Aman_boy/AnimationInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\01.KPUFinalProject\The Eternals\FrameDirectX12\Bin\Resource\ResourceStage\DynamicMesh\NPC\Aman_boy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7B02DD-B7C5-430A-B3A7-FF5052FA147E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4ED859-AF64-4D30-A1B3-39C5736854EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20160" yWindow="160" windowWidth="19430" windowHeight="10430" xr2:uid="{61396BBF-947E-42B3-B422-339E63356C45}"/>
+    <workbookView xWindow="465" yWindow="1395" windowWidth="12675" windowHeight="11385" xr2:uid="{61396BBF-947E-42B3-B422-339E63356C45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Animation Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +60,14 @@
   </si>
   <si>
     <t>Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Laugh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3945F1B-935D-41F2-9305-F8AE345AF27E}">
-  <dimension ref="C3:F6"/>
+  <dimension ref="C3:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -527,6 +535,34 @@
         <v>182</v>
       </c>
     </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>183</v>
+      </c>
+      <c r="F7" s="1">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>329</v>
+      </c>
+      <c r="F8" s="1">
+        <v>471</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>